<commit_message>
User types set and structure
</commit_message>
<xml_diff>
--- a/MicroGrids/Results/Battery_Data.xlsx
+++ b/MicroGrids/Results/Battery_Data.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giulia\GitHub\MicroGridsPy-Teaching\MicroGrids\Results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFEB9CA-558D-47E6-8E61-BA535A2EAB45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Battery_Data" sheetId="1" r:id="rId1"/>
     <sheet name="Yearly BRC" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Nominal Capacity at upgrade 1</t>
   </si>
@@ -42,13 +36,67 @@
   </si>
   <si>
     <t>Battery Replacement Cost at y = 2</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 3</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 4</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 5</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 6</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 7</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 8</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 9</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 10</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 11</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 12</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 13</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 14</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 15</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 16</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 17</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 18</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 19</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,23 +155,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -165,7 +205,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -197,27 +237,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -249,24 +271,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -442,52 +446,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="B1" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.53158528266100002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2712216.28371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.39337310916913998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2007040.0499454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>7.8674621833828007E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40140.800998908</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.113355856262</v>
+        <v>664663.574098</v>
       </c>
     </row>
   </sheetData>
@@ -496,36 +496,176 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>5.668131650166288E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47443.72683102623</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3">
-        <v>5.6674539760673173E-2</v>
+        <v>47632.94166258632</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>47618.10862433855</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>47619.97206547673</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>47624.80395492163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>47627.06485060284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>47628.36621991211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>47629.33247145954</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>47630.27460722077</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>47631.21703531164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>47632.18524322069</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>47633.22584214556</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>47634.17763780378</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>47635.27687057104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>47636.40274215503</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>47637.68278665161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>47638.98149000909</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>47640.27735621159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>47641.43246232736</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>47600.21489230519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More patching in Results
</commit_message>
<xml_diff>
--- a/MicroGrids/Results/Battery_Data.xlsx
+++ b/MicroGrids/Results/Battery_Data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Nominal Capacity at upgrade 1</t>
   </si>
@@ -45,51 +45,6 @@
   </si>
   <si>
     <t>Battery Replacement Cost at y = 5</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 6</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 7</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 8</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 9</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 10</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 11</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 12</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 13</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 14</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 15</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 16</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 17</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 18</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 19</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 20</t>
   </si>
 </sst>
 </file>
@@ -463,7 +418,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>2712216.28371</v>
+        <v>961.4826571789999</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -471,7 +426,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2007040.0499454</v>
+        <v>711.49716631246</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -479,7 +434,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>40140.800998908</v>
+        <v>14.2299433262492</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -487,7 +442,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>664663.574098</v>
+        <v>118.668407446</v>
       </c>
     </row>
   </sheetData>
@@ -497,7 +452,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -513,7 +468,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>47443.72683102623</v>
+        <v>25.31201466157464</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -521,7 +476,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>47632.94166258632</v>
+        <v>25.87534405914255</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -529,7 +484,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>47618.10862433855</v>
+        <v>26.44599501734016</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -537,7 +492,7 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>47619.97206547673</v>
+        <v>27.03532082871376</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -545,127 +500,7 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>47624.80395492163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>47627.06485060284</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>47628.36621991211</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>47629.33247145954</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <v>47630.27460722077</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>47631.21703531164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>47632.18524322069</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13">
-        <v>47633.22584214556</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
-        <v>47634.17763780378</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15">
-        <v>47635.27687057104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16">
-        <v>47636.40274215503</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17">
-        <v>47637.68278665161</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18">
-        <v>47638.98149000909</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19">
-        <v>47640.27735621159</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20">
-        <v>47641.43246232736</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21">
-        <v>47600.21489230519</v>
+        <v>27.70666213424036</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Third run HL, test
5% llp for just heavy load (user classes 5-8)
</commit_message>
<xml_diff>
--- a/MicroGrids/Results/Battery_Data.xlsx
+++ b/MicroGrids/Results/Battery_Data.xlsx
@@ -415,7 +415,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5653.47416886</v>
+        <v>10905.3054173</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -423,7 +423,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>565.347416886</v>
+        <v>1090.53054173</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -431,7 +431,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>11.30694833772</v>
+        <v>21.8106108346</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -439,7 +439,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>17.7844600346</v>
+        <v>34.1708264287</v>
       </c>
     </row>
   </sheetData>
@@ -465,7 +465,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>4.865122758888848</v>
+        <v>9.351160844696535</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -473,7 +473,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>4.86360170119019</v>
+        <v>9.344859523693639</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -481,7 +481,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>4.864784102044671</v>
+        <v>9.345878495719571</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -489,7 +489,7 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>4.865951861948579</v>
+        <v>9.346908547154163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First project output + confirm fix
To be tested with non user differentiated version and same inputs
</commit_message>
<xml_diff>
--- a/MicroGrids/Results/Battery_Data.xlsx
+++ b/MicroGrids/Results/Battery_Data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Nominal Capacity at upgrade 1</t>
   </si>
@@ -42,6 +42,54 @@
   </si>
   <si>
     <t>Battery Replacement Cost at y = 4</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 5</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 6</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 7</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 8</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 9</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 10</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 11</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 12</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 13</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 14</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 15</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 16</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 17</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 18</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 19</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 20</t>
   </si>
 </sst>
 </file>
@@ -415,7 +463,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>10905.3054173</v>
+        <v>26.0753354553</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -423,7 +471,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1090.53054173</v>
+        <v>14.080681145862</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -431,7 +479,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>21.8106108346</v>
+        <v>0.28161362291724</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -439,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>34.1708264287</v>
+        <v>4.97494874334</v>
       </c>
     </row>
   </sheetData>
@@ -449,7 +497,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -465,7 +513,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>9.351160844696535</v>
+        <v>0.6286452380429166</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -473,7 +521,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>9.344859523693639</v>
+        <v>0.6433874021842154</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -481,7 +529,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>9.345878495719571</v>
+        <v>0.6606993624998114</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -489,7 +537,135 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>9.346908547154163</v>
+        <v>0.6806390408598679</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>0.7038081714019271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>0.730752324459822</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0.7616039398545558</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0.7965992632711851</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>0.836035758905422</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>0.8803156244852249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>0.9299165750643577</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>0.9853259660240716</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>1.047170289693914</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>1.11597647473226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>1.191990881979759</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>1.27511091357169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>1.364759030235794</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>1.459724038914086</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>1.558547236289639</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>1.65975115358533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First project output, test
</commit_message>
<xml_diff>
--- a/MicroGrids/Results/Battery_Data.xlsx
+++ b/MicroGrids/Results/Battery_Data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Nominal Capacity at upgrade 1</t>
   </si>
@@ -42,6 +42,54 @@
   </si>
   <si>
     <t>Battery Replacement Cost at y = 4</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 5</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 6</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 7</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 8</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 9</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 10</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 11</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 12</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 13</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 14</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 15</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 16</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 17</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 18</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 19</t>
+  </si>
+  <si>
+    <t>Battery Replacement Cost at y = 20</t>
   </si>
 </sst>
 </file>
@@ -415,7 +463,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5059.58333458</v>
+        <v>34.3685988048</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -423,7 +471,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>505.958333458</v>
+        <v>18.559043354592</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -431,7 +479,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>10.11916666916</v>
+        <v>0.3711808670918401</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -439,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>15.8437082613</v>
+        <v>6.37166537488</v>
       </c>
     </row>
   </sheetData>
@@ -449,7 +497,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -465,7 +513,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>4.334713039182466</v>
+        <v>0.7982541322620772</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -473,7 +521,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>4.333205517307831</v>
+        <v>0.81737474436244</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -481,7 +529,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>4.333714978622995</v>
+        <v>0.8383750009946094</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -489,7 +537,135 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>4.334211386930692</v>
+        <v>0.8620796584972996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>0.8897504170499579</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>0.9225060407143506</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0.9619115834189335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>1.0095103835637</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>1.06531849117498</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>1.129309976919592</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>1.201802342693103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>1.282820757874964</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>1.372014508240509</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>1.468652028395985</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>1.572213123728664</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>1.682267726638863</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>1.798366570241442</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>1.919892149598082</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>2.045897355990393</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>2.175136961007468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Results, scenario business, min OC
</commit_message>
<xml_diff>
--- a/MicroGrids/Results/Battery_Data.xlsx
+++ b/MicroGrids/Results/Battery_Data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Nominal Capacity at upgrade 1</t>
   </si>
@@ -30,12 +30,6 @@
   </si>
   <si>
     <t>Scenario 1</t>
-  </si>
-  <si>
-    <t>Scenario 2</t>
-  </si>
-  <si>
-    <t>Scenario 3</t>
   </si>
   <si>
     <t>Battery Replacement Cost at y = 1</t>
@@ -469,7 +463,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>259044.241780225</v>
+        <v>533086.236485</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -477,7 +471,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>139883.8905613215</v>
+        <v>287866.5677019</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -485,7 +479,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2797.677811226431</v>
+        <v>5757.331354038</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -493,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>22569.2807412759</v>
+        <v>73055.0735398</v>
       </c>
     </row>
   </sheetData>
@@ -503,301 +497,175 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2">
+        <v>8901.973929389769</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="B3">
+        <v>8921.293601269652</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>813.3990115005738</v>
-      </c>
-      <c r="C2">
-        <v>816.9982519286134</v>
-      </c>
-      <c r="D2">
-        <v>820.9283312715581</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+      <c r="B4">
+        <v>11037.67942807288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>3145.339385449878</v>
-      </c>
-      <c r="C3">
-        <v>2938.864796429967</v>
-      </c>
-      <c r="D3">
-        <v>2937.814805138287</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
+      <c r="B5">
+        <v>11035.38907423939</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>3583.893438081187</v>
-      </c>
-      <c r="C4">
-        <v>3362.337698442338</v>
-      </c>
-      <c r="D4">
-        <v>3365.398578036028</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
+      <c r="B6">
+        <v>11035.41157114427</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
-        <v>3586.304659475069</v>
-      </c>
-      <c r="C5">
-        <v>3364.69934411282</v>
-      </c>
-      <c r="D5">
-        <v>3367.763819396321</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
+      <c r="B7">
+        <v>11035.15215792765</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
-        <v>3586.305783202875</v>
-      </c>
-      <c r="C6">
-        <v>3364.700264443266</v>
-      </c>
-      <c r="D6">
-        <v>3367.76481353097</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
+      <c r="B8">
+        <v>11036.31439383162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
-        <v>3586.306869396903</v>
-      </c>
-      <c r="C7">
-        <v>3364.701787402248</v>
-      </c>
-      <c r="D7">
-        <v>3367.766479987552</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
+      <c r="B9">
+        <v>14754.89891929362</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>3586.481849561156</v>
-      </c>
-      <c r="C8">
-        <v>3367.042858976866</v>
-      </c>
-      <c r="D8">
-        <v>3370.381216404285</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
+      <c r="B10">
+        <v>14761.2444396714</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
-        <v>4052.989081731507</v>
-      </c>
-      <c r="C9">
-        <v>4972.415348534829</v>
-      </c>
-      <c r="D9">
-        <v>4937.635841776726</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
+      <c r="B11">
+        <v>14759.92952075165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
-        <v>4055.670529129067</v>
-      </c>
-      <c r="C10">
-        <v>4978.383550619401</v>
-      </c>
-      <c r="D10">
-        <v>4943.454482568099</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
+      <c r="B12">
+        <v>14759.93231987803</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
-        <v>4055.670944977392</v>
-      </c>
-      <c r="C11">
-        <v>4978.3992241297</v>
-      </c>
-      <c r="D11">
-        <v>4943.470430636406</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
+      <c r="B13">
+        <v>14759.93186743955</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12">
-        <v>4055.670946102567</v>
-      </c>
-      <c r="C12">
-        <v>4978.399230315927</v>
-      </c>
-      <c r="D12">
-        <v>4943.470442377913</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
+      <c r="B14">
+        <v>14759.85803017142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
-        <v>4055.670943162901</v>
-      </c>
-      <c r="C13">
-        <v>4978.399273471795</v>
-      </c>
-      <c r="D13">
-        <v>4943.470499439363</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
+      <c r="B15">
+        <v>14756.93226478668</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
-        <v>4055.667534661588</v>
-      </c>
-      <c r="C14">
-        <v>4978.397958012136</v>
-      </c>
-      <c r="D14">
-        <v>4943.47335302851</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
+      <c r="B16">
+        <v>14041.06698898696</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B15">
-        <v>4062.111073399787</v>
-      </c>
-      <c r="C15">
-        <v>4976.275101275369</v>
-      </c>
-      <c r="D15">
-        <v>4941.707145372431</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1" t="s">
+      <c r="B17">
+        <v>14045.13175366128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16">
-        <v>4815.550799774963</v>
-      </c>
-      <c r="C16">
-        <v>7681.798268418823</v>
-      </c>
-      <c r="D16">
-        <v>7647.560219354498</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1" t="s">
+      <c r="B18">
+        <v>14045.18489499017</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B17">
-        <v>4818.868120345734</v>
-      </c>
-      <c r="C17">
-        <v>7681.306485897754</v>
-      </c>
-      <c r="D17">
-        <v>7646.969801748153</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1" t="s">
+      <c r="B19">
+        <v>14045.18031908991</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18">
-        <v>4818.87384867925</v>
-      </c>
-      <c r="C18">
-        <v>7681.31129887285</v>
-      </c>
-      <c r="D18">
-        <v>7646.969202566375</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1" t="s">
+      <c r="B20">
+        <v>14045.29781027313</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B19">
-        <v>4818.877557806198</v>
-      </c>
-      <c r="C19">
-        <v>7681.312456282339</v>
-      </c>
-      <c r="D19">
-        <v>7646.96874467323</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20">
-        <v>4820.134979504701</v>
-      </c>
-      <c r="C20">
-        <v>7680.925831590661</v>
-      </c>
-      <c r="D20">
-        <v>7646.836599926349</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="B21">
-        <v>5074.151734348938</v>
-      </c>
-      <c r="C21">
-        <v>7651.846799067048</v>
-      </c>
-      <c r="D21">
-        <v>7639.176302275453</v>
+        <v>14043.04247608956</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Yearly limit removed + results same scenario as previous commit
</commit_message>
<xml_diff>
--- a/MicroGrids/Results/Battery_Data.xlsx
+++ b/MicroGrids/Results/Battery_Data.xlsx
@@ -463,7 +463,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>533086.236485</v>
+        <v>532808.278649</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -471,7 +471,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>287866.5677019</v>
+        <v>287716.47047046</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -479,7 +479,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5757.331354038</v>
+        <v>5754.329409409201</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -487,7 +487,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>73055.0735398</v>
+        <v>72986.98354080001</v>
       </c>
     </row>
   </sheetData>
@@ -513,7 +513,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>8901.973929389769</v>
+        <v>8893.01839920877</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -521,7 +521,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>8921.293601269652</v>
+        <v>8911.786229106507</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -529,7 +529,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>11037.67942807288</v>
+        <v>11024.66356877324</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -537,7 +537,7 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>11035.38907423939</v>
+        <v>11024.87703796586</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -545,7 +545,7 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>11035.41157114427</v>
+        <v>11024.87703796586</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -553,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>11035.15215792765</v>
+        <v>11024.87703796586</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -561,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>11036.31439383162</v>
+        <v>11021.40227621262</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -569,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>14754.89891929362</v>
+        <v>14751.75318293285</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -577,7 +577,7 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>14761.2444396714</v>
+        <v>14747.52888169423</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -585,7 +585,7 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>14759.92952075165</v>
+        <v>14747.52888169423</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -593,7 +593,7 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>14759.93231987803</v>
+        <v>14747.52888169423</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -601,7 +601,7 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>14759.93186743955</v>
+        <v>14747.52888169423</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -609,7 +609,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>14759.85803017142</v>
+        <v>14747.52888169423</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -617,7 +617,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>14756.93226478668</v>
+        <v>14742.7237413523</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -625,7 +625,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>14041.06698898696</v>
+        <v>14029.60553099276</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -633,7 +633,7 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>14045.13175366128</v>
+        <v>14033.3818769272</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -641,7 +641,7 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>14045.18489499017</v>
+        <v>14033.3818769272</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -649,7 +649,7 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>14045.18031908991</v>
+        <v>14033.3818769272</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -657,7 +657,7 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>14045.29781027313</v>
+        <v>14033.38187692721</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -665,7 +665,7 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>14043.04247608956</v>
+        <v>14031.2710065673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Important fix + cooking demand
Also a script that automatically generates waste supply excel
</commit_message>
<xml_diff>
--- a/MicroGrids/Results/Battery_Data.xlsx
+++ b/MicroGrids/Results/Battery_Data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Nominal Capacity at upgrade 1</t>
   </si>
@@ -32,12 +32,6 @@
     <t>Scenario 1</t>
   </si>
   <si>
-    <t>Scenario 2</t>
-  </si>
-  <si>
-    <t>Scenario 3</t>
-  </si>
-  <si>
     <t>Battery Replacement Cost at y = 1</t>
   </si>
   <si>
@@ -51,51 +45,6 @@
   </si>
   <si>
     <t>Battery Replacement Cost at y = 5</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 6</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 7</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 8</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 9</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 10</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 11</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 12</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 13</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 14</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 15</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 16</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 17</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 18</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 19</t>
-  </si>
-  <si>
-    <t>Battery Replacement Cost at y = 20</t>
   </si>
 </sst>
 </file>
@@ -469,7 +418,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>503872.9332211489</v>
+        <v>477169.308357</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -477,7 +426,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>272091.3839394205</v>
+        <v>257671.42651278</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -485,7 +434,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5441.827678788409</v>
+        <v>5153.428530255601</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -493,7 +442,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>44462.83149052429</v>
+        <v>23171.2993725</v>
       </c>
     </row>
   </sheetData>
@@ -503,301 +452,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2">
+        <v>5854.494437752516</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="B3">
+        <v>7089.738675278473</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>5904.819777969491</v>
-      </c>
-      <c r="C2">
-        <v>5902.831121983219</v>
-      </c>
-      <c r="D2">
-        <v>5857.25035399163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+      <c r="B4">
+        <v>7085.67074441673</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>5915.232817136706</v>
-      </c>
-      <c r="C3">
-        <v>5913.066406523016</v>
-      </c>
-      <c r="D3">
-        <v>5867.50278742019</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
+      <c r="B5">
+        <v>7854.817185727328</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>7106.410704171727</v>
-      </c>
-      <c r="C4">
-        <v>7138.174235220064</v>
-      </c>
-      <c r="D4">
-        <v>7094.719455175066</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>7105.336844353524</v>
-      </c>
-      <c r="C5">
-        <v>7136.878984523482</v>
-      </c>
-      <c r="D5">
-        <v>7093.457592054974</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="B6">
-        <v>7105.336844333396</v>
-      </c>
-      <c r="C6">
-        <v>7136.878984509596</v>
-      </c>
-      <c r="D6">
-        <v>7093.457592039671</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>7105.336844333802</v>
-      </c>
-      <c r="C7">
-        <v>7136.878984510278</v>
-      </c>
-      <c r="D7">
-        <v>7093.457592040066</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8">
-        <v>7104.740919734574</v>
-      </c>
-      <c r="C8">
-        <v>7135.045217970788</v>
-      </c>
-      <c r="D8">
-        <v>7091.404952266313</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>8004.825297765703</v>
-      </c>
-      <c r="C9">
-        <v>8184.17528630132</v>
-      </c>
-      <c r="D9">
-        <v>8119.399313003623</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>8004.383011310018</v>
-      </c>
-      <c r="C10">
-        <v>8181.560062596446</v>
-      </c>
-      <c r="D10">
-        <v>8116.706265759279</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
-        <v>8004.383011316967</v>
-      </c>
-      <c r="C11">
-        <v>8181.560062626645</v>
-      </c>
-      <c r="D11">
-        <v>8116.706265790757</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <v>8004.383011316957</v>
-      </c>
-      <c r="C12">
-        <v>8181.560062626644</v>
-      </c>
-      <c r="D12">
-        <v>8116.706265790743</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <v>8004.383011316971</v>
-      </c>
-      <c r="C13">
-        <v>8181.560062626655</v>
-      </c>
-      <c r="D13">
-        <v>8116.706265790757</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14">
-        <v>8004.3830113172</v>
-      </c>
-      <c r="C14">
-        <v>8181.560062626023</v>
-      </c>
-      <c r="D14">
-        <v>8116.706265789826</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15">
-        <v>8003.701319768488</v>
-      </c>
-      <c r="C15">
-        <v>8177.911149387382</v>
-      </c>
-      <c r="D15">
-        <v>8112.820685188644</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16">
-        <v>8344.719839245547</v>
-      </c>
-      <c r="C16">
-        <v>7611.765359871755</v>
-      </c>
-      <c r="D16">
-        <v>7504.050977463612</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17">
-        <v>8343.511413817734</v>
-      </c>
-      <c r="C17">
-        <v>7616.029538403858</v>
-      </c>
-      <c r="D17">
-        <v>7508.595396874338</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18">
-        <v>8343.511413836193</v>
-      </c>
-      <c r="C18">
-        <v>7616.029538371418</v>
-      </c>
-      <c r="D18">
-        <v>7508.595396928478</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19">
-        <v>8343.511413836106</v>
-      </c>
-      <c r="C19">
-        <v>7616.02953837217</v>
-      </c>
-      <c r="D19">
-        <v>7508.595396928452</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20">
-        <v>8343.511413727168</v>
-      </c>
-      <c r="C20">
-        <v>7616.029540005113</v>
-      </c>
-      <c r="D20">
-        <v>7508.595396932998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21">
-        <v>8345.465424111924</v>
-      </c>
-      <c r="C21">
-        <v>7614.781722734095</v>
-      </c>
-      <c r="D21">
-        <v>7507.275068796784</v>
+        <v>7179.766543521098</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned inputs + important changes
</commit_message>
<xml_diff>
--- a/MicroGrids/Results/Battery_Data.xlsx
+++ b/MicroGrids/Results/Battery_Data.xlsx
@@ -418,7 +418,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>477169.308357</v>
+        <v>406638.746988</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -426,7 +426,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>257671.42651278</v>
+        <v>219584.92337352</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -434,7 +434,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5153.428530255601</v>
+        <v>4391.698467470401</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -442,7 +442,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>23171.2993725</v>
+        <v>21683.1714275</v>
       </c>
     </row>
   </sheetData>
@@ -468,7 +468,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>5854.494437752516</v>
+        <v>5850.092220579987</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -476,7 +476,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>7089.738675278473</v>
+        <v>6936.583990863766</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -484,7 +484,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>7085.67074441673</v>
+        <v>6933.451650374368</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -492,7 +492,7 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>7854.817185727328</v>
+        <v>6621.112361776992</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -500,7 +500,7 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>7179.766543521098</v>
+        <v>6047.308640889105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>